<commit_message>
SW modified name on Captains Contact
</commit_message>
<xml_diff>
--- a/secure/captains-contact2019.xlsx
+++ b/secure/captains-contact2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\OneDrive\BCG-Zone-4\secure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CCF058-3E27-4092-B114-6CFC70D33471}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8F6CEA-0114-4120-8474-B5665498DC5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="2115" windowWidth="11760" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7620" yWindow="2475" windowWidth="19890" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
   <si>
     <t>WOMEN’S ZONE 4 CLUB ROSTER</t>
   </si>
@@ -273,39 +273,6 @@
     <t>February, 2019</t>
   </si>
   <si>
-    <t>Nora Thomas</t>
-  </si>
-  <si>
-    <t>norathithomas@gmail.com</t>
-  </si>
-  <si>
-    <t>Ann Watson</t>
-  </si>
-  <si>
-    <t>604-885-0739</t>
-  </si>
-  <si>
-    <t>annwatson@dcc.net.com</t>
-  </si>
-  <si>
-    <t>Sheila McArthur</t>
-  </si>
-  <si>
-    <t>604-947-0444</t>
-  </si>
-  <si>
-    <t>shemac95@shaw.ca</t>
-  </si>
-  <si>
-    <t>Caryl Nelson</t>
-  </si>
-  <si>
-    <t>604-939-6318</t>
-  </si>
-  <si>
-    <t>carylnelson@shaw.ca</t>
-  </si>
-  <si>
     <t>Kathy Appleby</t>
   </si>
   <si>
@@ -490,6 +457,42 @@
   </si>
   <si>
     <t>2019 CAPTAIN’S LIST</t>
+  </si>
+  <si>
+    <t>Sherry Whitman</t>
+  </si>
+  <si>
+    <t>604 831 9864</t>
+  </si>
+  <si>
+    <t>swhitman49@gmail.com</t>
+  </si>
+  <si>
+    <t>Chris Twaits</t>
+  </si>
+  <si>
+    <t>604-989-7171</t>
+  </si>
+  <si>
+    <t>ctwaits55@gmail.com</t>
+  </si>
+  <si>
+    <t>Barb Rendell</t>
+  </si>
+  <si>
+    <t>604-947-0838</t>
+  </si>
+  <si>
+    <t>rgmiller38@icloud.com</t>
+  </si>
+  <si>
+    <t>Lily Fan</t>
+  </si>
+  <si>
+    <t>604-421-1095</t>
+  </si>
+  <si>
+    <t>lfan1688@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -613,15 +616,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -655,19 +649,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -771,6 +752,77 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -778,7 +830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -795,84 +847,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1309,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection sqref="A1:E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A1:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,31 +1384,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="32"/>
+      <c r="B1" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
-      <c r="B3" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1356,174 +1417,176 @@
       <c r="B4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="23" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40" t="s">
+      <c r="D9" s="31" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="39" t="s">
+      <c r="E9" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="39" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="D10" s="24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="39" t="s">
+      <c r="E10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="20" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="27" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="5"/>
+      <c r="C12" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="24"/>
       <c r="E12" s="41"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="20" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="20" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1532,14 +1595,14 @@
         <v>16</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>102</v>
+      <c r="C16" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1547,360 +1610,360 @@
         <v>78</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="25" t="s">
-        <v>103</v>
+      <c r="E17" s="20" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>106</v>
+      <c r="C18" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>110</v>
+      <c r="C19" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="12" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="20" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="27" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>113</v>
+      <c r="C22" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="11" t="s">
+      <c r="A23" s="28"/>
+      <c r="B23" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>116</v>
+      <c r="C23" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="13" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="C24" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
         <v>71</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>122</v>
+      <c r="C26" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>125</v>
+      <c r="C27" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="6"/>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="25" t="s">
-        <v>126</v>
+      <c r="E28" s="20" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="6"/>
-      <c r="C29" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>129</v>
+      <c r="C29" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="14" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="D36" s="24" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="14" t="s">
+      <c r="E36" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="27" t="s">
         <v>73</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="E37" s="19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E38" s="25" t="s">
-        <v>147</v>
+        <v>135</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="27" t="s">
         <v>45</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>66</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>150</v>
+        <v>138</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="6" t="s">
         <v>65</v>
       </c>
@@ -1910,42 +1973,42 @@
       <c r="D40" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="25" t="s">
+      <c r="E40" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>153</v>
+        <v>141</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="21" t="s">
+      <c r="B42" s="15"/>
+      <c r="C42" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="21" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="17" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1964,44 +2027,46 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E37" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E10" r:id="rId3" display="bawagner@shaw.ca" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E16" r:id="rId8" display="sandy_harvell@yahoo.com" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E18" r:id="rId9" display="brandpat@telus.net" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E21" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E22" r:id="rId12" display="dchoag@shaw.ca" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E23" r:id="rId13" display="jeannebye@shaw.ca" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E24" r:id="rId14" display="dianemcneely8@gmail.com" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E25" r:id="rId15" display="esthercaldes@gmail.com" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E26" r:id="rId16" display="scooterlady@telus.net" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E27" r:id="rId17" display="carollacroix@hotmail.com" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E28" r:id="rId18" display="glenbrookhomes@dcc.net.com" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E29" r:id="rId19" display="joanproudfoot@gmail.com" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E30" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E32" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E33" r:id="rId22" display="jo4ygea@gmail.com" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="E34" r:id="rId23" display="henriksen7@gmail.com" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E35" r:id="rId24" display="bla8873@telus.net" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E36" r:id="rId25" display="bevdrombolis@gmail.com" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="E38" r:id="rId26" display="moira.milligan@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E39" r:id="rId27" display="Lindai@shaw.ca" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="E40" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E41" r:id="rId29" display="barriemose@gmail.com" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E42" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="E17" r:id="rId31" display="margmacsuch@gmail.com" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E5" r:id="rId32" xr:uid="{928410D7-B706-4594-8CA4-CC5E14540209}"/>
-    <hyperlink ref="E6" r:id="rId33" xr:uid="{F35EA726-1C12-4D00-B2AA-6AD84933F7AB}"/>
-    <hyperlink ref="E7" r:id="rId34" xr:uid="{9660795F-5E9B-435B-A545-0DCBC785F7C7}"/>
-    <hyperlink ref="E8" r:id="rId35" xr:uid="{7C7C6C0D-5D8B-4513-90D3-1D9E93B9E03D}"/>
+    <hyperlink ref="E38" r:id="rId2" display="moira.milligan@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E39" r:id="rId3" display="Lindai@shaw.ca" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E40" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E41" r:id="rId5" display="barriemose@gmail.com" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E42" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{E73A42E7-4F8F-4D5E-B8D5-E02F6AAE39AB}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{6654D1FF-77EA-453B-BF40-0E665FAFE727}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{6C1D7C9A-D442-4F8E-931C-2B79D2276A12}"/>
+    <hyperlink ref="E8" r:id="rId10" xr:uid="{F6528273-553B-4CDF-8CD7-DC6EB56ABC74}"/>
+    <hyperlink ref="E9" r:id="rId11" xr:uid="{8CAB84D4-83CF-40C4-9AEA-84B32BB82E86}"/>
+    <hyperlink ref="E10" r:id="rId12" xr:uid="{3F569760-7D85-4889-9102-B74CBE96E830}"/>
+    <hyperlink ref="E11" r:id="rId13" xr:uid="{C22C70E3-74A2-4A57-9F13-73D75A6DDE2A}"/>
+    <hyperlink ref="E13" r:id="rId14" xr:uid="{88A26EFE-CFAE-4784-A0FE-92E84C720A0E}"/>
+    <hyperlink ref="E14" r:id="rId15" xr:uid="{7F958C3B-165B-4E92-9C55-7353C576DAA1}"/>
+    <hyperlink ref="E15" r:id="rId16" xr:uid="{82E76F6A-8BCE-444F-A364-6DB6F8514B70}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{77149E56-D3B0-4D9F-8AC3-3F9A93E3B552}"/>
+    <hyperlink ref="E17" r:id="rId18" xr:uid="{1A90BE41-E0DD-4EF9-823B-CFD5CF11644A}"/>
+    <hyperlink ref="E18" r:id="rId19" xr:uid="{66F84E1C-03B4-4719-ADFA-05868C261C15}"/>
+    <hyperlink ref="E19" r:id="rId20" xr:uid="{2F02FF80-425A-410D-B418-596DB0B2831C}"/>
+    <hyperlink ref="E20" r:id="rId21" xr:uid="{F5533712-EFBF-482D-938F-B3C3B9F6115F}"/>
+    <hyperlink ref="E21" r:id="rId22" xr:uid="{6E26E6B4-40D5-4F23-9A68-BB39316F8862}"/>
+    <hyperlink ref="E22" r:id="rId23" xr:uid="{6BB8B619-18FD-4E8F-8BC4-15C168708406}"/>
+    <hyperlink ref="E23" r:id="rId24" xr:uid="{051527AE-517F-4321-B66C-C5346350E949}"/>
+    <hyperlink ref="E24" r:id="rId25" xr:uid="{851B2E8B-6590-4449-BDE8-F99844E1993A}"/>
+    <hyperlink ref="E25" r:id="rId26" xr:uid="{48A2305D-AC47-4859-91E5-CBB72DD4C293}"/>
+    <hyperlink ref="E26" r:id="rId27" xr:uid="{69CCAEE5-9782-4D21-A16E-F587EECCC910}"/>
+    <hyperlink ref="E27" r:id="rId28" xr:uid="{183EC305-E441-4C2F-B433-5A4F34BFB887}"/>
+    <hyperlink ref="E28" r:id="rId29" xr:uid="{9AD4EEA4-4CCC-47AE-B297-0C881EEBA412}"/>
+    <hyperlink ref="E29" r:id="rId30" xr:uid="{361CD294-D9C9-48DE-B360-FAEAF0912D81}"/>
+    <hyperlink ref="E30" r:id="rId31" xr:uid="{7727B2F8-9B9F-462A-BCEE-52B7B2945198}"/>
+    <hyperlink ref="E31" r:id="rId32" xr:uid="{33E37E03-5009-434C-A3E8-5850F7097F4B}"/>
+    <hyperlink ref="E32" r:id="rId33" xr:uid="{42977E3D-9090-47F4-B380-9D2224403F81}"/>
+    <hyperlink ref="E33" r:id="rId34" xr:uid="{38B980A3-571A-414E-91A7-553B9E547FB4}"/>
+    <hyperlink ref="E34" r:id="rId35" xr:uid="{E693AF38-7F54-46F6-B4DA-84396E3BA38E}"/>
+    <hyperlink ref="E35" r:id="rId36" xr:uid="{2BCCBA48-D686-4ACA-9CCF-B66E1F8230BF}"/>
+    <hyperlink ref="E36" r:id="rId37" xr:uid="{F96302C6-F783-4E95-B61D-C103629E9C81}"/>
   </hyperlinks>
   <pageMargins left="0.4" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
-  <drawing r:id="rId37"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
+  <drawing r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SW added Marine Drive to Roster & Captains
</commit_message>
<xml_diff>
--- a/secure/captains-contact2019.xlsx
+++ b/secure/captains-contact2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8F6CEA-0114-4120-8474-B5665498DC5A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3772FA-C1C0-4667-A4BE-BC5CF777D8A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="2475" windowWidth="19890" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2415" yWindow="3345" windowWidth="19890" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$44</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="158">
   <si>
     <t>WOMEN’S ZONE 4 CLUB ROSTER</t>
   </si>
@@ -87,9 +87,6 @@
     <t>604-306-3939</t>
   </si>
   <si>
-    <t>marjallen@me.com</t>
-  </si>
-  <si>
     <t>Mayfair</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Marj Allen</t>
-  </si>
-  <si>
     <t>Club</t>
   </si>
   <si>
@@ -493,13 +487,25 @@
   </si>
   <si>
     <t>lfan1688@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheryl Khanna </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carrie Cade </t>
+  </si>
+  <si>
+    <t>cherylkhanna1@gmail.com</t>
+  </si>
+  <si>
+    <t>cadeclm@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,6 +544,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -553,7 +565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -823,6 +835,19 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -830,7 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -875,55 +900,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -934,6 +917,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1368,10 +1396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A1:E43"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,47 +1412,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="39"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>55</v>
+        <v>66</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,14 +1460,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>144</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,14 +1475,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1462,14 +1490,14 @@
         <v>3</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1477,14 +1505,14 @@
         <v>4</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>153</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1492,14 +1520,14 @@
         <v>5</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>82</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1507,14 +1535,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>85</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1522,42 +1550,42 @@
         <v>7</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="E13" s="20" t="s">
         <v>60</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1565,10 +1593,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="20" t="s">
@@ -1580,10 +1608,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="20" t="s">
@@ -1591,33 +1619,33 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="24" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="20" t="s">
         <v>90</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1625,413 +1653,426 @@
         <v>17</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="24" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="B19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="23" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+      <c r="D19" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="E19" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="24" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="D23" s="23" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="20" t="s">
+      <c r="E23" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="40"/>
+      <c r="B24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="24" t="s">
+      <c r="D26" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="41"/>
+      <c r="B27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="D27" s="23" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="24" t="s">
+      <c r="E27" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="24" t="s">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="40"/>
+      <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="D28" s="23" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="24" t="s">
+      <c r="E28" s="20" t="s">
         <v>112</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" s="24" t="s">
+      <c r="B31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="40"/>
+      <c r="B32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="D32" s="23" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="24" t="s">
+      <c r="E32" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="D31" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B33" s="6"/>
-      <c r="C33" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>123</v>
+      <c r="C33" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6"/>
-      <c r="C34" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>126</v>
+      <c r="C34" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>121</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" s="6"/>
-      <c r="C35" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>129</v>
+      <c r="C35" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>124</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="40"/>
+      <c r="B39" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="B40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="D40" s="5" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="E40" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="40"/>
+      <c r="B41" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="D41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="D42" s="5" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="E42" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+      <c r="B43" s="15"/>
+      <c r="C43" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="16" t="s">
+      <c r="D43" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="E43" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>74</v>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="17" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E37" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E38" r:id="rId2" display="moira.milligan@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E39" r:id="rId3" display="Lindai@shaw.ca" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="E40" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E41" r:id="rId5" display="barriemose@gmail.com" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E42" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="E38" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E39" r:id="rId2" display="moira.milligan@gmail.com" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E40" r:id="rId3" display="Lindai@shaw.ca" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="E41" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E42" r:id="rId5" display="barriemose@gmail.com" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E43" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
     <hyperlink ref="E5" r:id="rId7" xr:uid="{E73A42E7-4F8F-4D5E-B8D5-E02F6AAE39AB}"/>
     <hyperlink ref="E6" r:id="rId8" xr:uid="{6654D1FF-77EA-453B-BF40-0E665FAFE727}"/>
     <hyperlink ref="E7" r:id="rId9" xr:uid="{6C1D7C9A-D442-4F8E-931C-2B79D2276A12}"/>
@@ -2046,23 +2087,23 @@
     <hyperlink ref="E17" r:id="rId18" xr:uid="{1A90BE41-E0DD-4EF9-823B-CFD5CF11644A}"/>
     <hyperlink ref="E18" r:id="rId19" xr:uid="{66F84E1C-03B4-4719-ADFA-05868C261C15}"/>
     <hyperlink ref="E19" r:id="rId20" xr:uid="{2F02FF80-425A-410D-B418-596DB0B2831C}"/>
-    <hyperlink ref="E20" r:id="rId21" xr:uid="{F5533712-EFBF-482D-938F-B3C3B9F6115F}"/>
-    <hyperlink ref="E21" r:id="rId22" xr:uid="{6E26E6B4-40D5-4F23-9A68-BB39316F8862}"/>
-    <hyperlink ref="E22" r:id="rId23" xr:uid="{6BB8B619-18FD-4E8F-8BC4-15C168708406}"/>
-    <hyperlink ref="E23" r:id="rId24" xr:uid="{051527AE-517F-4321-B66C-C5346350E949}"/>
-    <hyperlink ref="E24" r:id="rId25" xr:uid="{851B2E8B-6590-4449-BDE8-F99844E1993A}"/>
-    <hyperlink ref="E25" r:id="rId26" xr:uid="{48A2305D-AC47-4859-91E5-CBB72DD4C293}"/>
-    <hyperlink ref="E26" r:id="rId27" xr:uid="{69CCAEE5-9782-4D21-A16E-F587EECCC910}"/>
-    <hyperlink ref="E27" r:id="rId28" xr:uid="{183EC305-E441-4C2F-B433-5A4F34BFB887}"/>
-    <hyperlink ref="E28" r:id="rId29" xr:uid="{9AD4EEA4-4CCC-47AE-B297-0C881EEBA412}"/>
-    <hyperlink ref="E29" r:id="rId30" xr:uid="{361CD294-D9C9-48DE-B360-FAEAF0912D81}"/>
-    <hyperlink ref="E30" r:id="rId31" xr:uid="{7727B2F8-9B9F-462A-BCEE-52B7B2945198}"/>
-    <hyperlink ref="E31" r:id="rId32" xr:uid="{33E37E03-5009-434C-A3E8-5850F7097F4B}"/>
-    <hyperlink ref="E32" r:id="rId33" xr:uid="{42977E3D-9090-47F4-B380-9D2224403F81}"/>
-    <hyperlink ref="E33" r:id="rId34" xr:uid="{38B980A3-571A-414E-91A7-553B9E547FB4}"/>
-    <hyperlink ref="E34" r:id="rId35" xr:uid="{E693AF38-7F54-46F6-B4DA-84396E3BA38E}"/>
-    <hyperlink ref="E35" r:id="rId36" xr:uid="{2BCCBA48-D686-4ACA-9CCF-B66E1F8230BF}"/>
-    <hyperlink ref="E36" r:id="rId37" xr:uid="{F96302C6-F783-4E95-B61D-C103629E9C81}"/>
+    <hyperlink ref="E20" r:id="rId21" display="marjallen@me.com" xr:uid="{F5533712-EFBF-482D-938F-B3C3B9F6115F}"/>
+    <hyperlink ref="E22" r:id="rId22" xr:uid="{6E26E6B4-40D5-4F23-9A68-BB39316F8862}"/>
+    <hyperlink ref="E23" r:id="rId23" xr:uid="{6BB8B619-18FD-4E8F-8BC4-15C168708406}"/>
+    <hyperlink ref="E24" r:id="rId24" xr:uid="{051527AE-517F-4321-B66C-C5346350E949}"/>
+    <hyperlink ref="E25" r:id="rId25" xr:uid="{851B2E8B-6590-4449-BDE8-F99844E1993A}"/>
+    <hyperlink ref="E26" r:id="rId26" xr:uid="{48A2305D-AC47-4859-91E5-CBB72DD4C293}"/>
+    <hyperlink ref="E27" r:id="rId27" xr:uid="{69CCAEE5-9782-4D21-A16E-F587EECCC910}"/>
+    <hyperlink ref="E28" r:id="rId28" xr:uid="{183EC305-E441-4C2F-B433-5A4F34BFB887}"/>
+    <hyperlink ref="E29" r:id="rId29" xr:uid="{9AD4EEA4-4CCC-47AE-B297-0C881EEBA412}"/>
+    <hyperlink ref="E30" r:id="rId30" xr:uid="{361CD294-D9C9-48DE-B360-FAEAF0912D81}"/>
+    <hyperlink ref="E31" r:id="rId31" xr:uid="{7727B2F8-9B9F-462A-BCEE-52B7B2945198}"/>
+    <hyperlink ref="E32" r:id="rId32" xr:uid="{33E37E03-5009-434C-A3E8-5850F7097F4B}"/>
+    <hyperlink ref="E33" r:id="rId33" xr:uid="{42977E3D-9090-47F4-B380-9D2224403F81}"/>
+    <hyperlink ref="E34" r:id="rId34" xr:uid="{38B980A3-571A-414E-91A7-553B9E547FB4}"/>
+    <hyperlink ref="E35" r:id="rId35" xr:uid="{E693AF38-7F54-46F6-B4DA-84396E3BA38E}"/>
+    <hyperlink ref="E36" r:id="rId36" xr:uid="{2BCCBA48-D686-4ACA-9CCF-B66E1F8230BF}"/>
+    <hyperlink ref="E37" r:id="rId37" xr:uid="{F96302C6-F783-4E95-B61D-C103629E9C81}"/>
   </hyperlinks>
   <pageMargins left="0.4" right="0.25" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId38"/>

</xml_diff>